<commit_message>
added Macbook test run results.
</commit_message>
<xml_diff>
--- a/assignment2/plot1Timings.xlsx
+++ b/assignment2/plot1Timings.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonard\gitrepos\ExData\assignment2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\GitHub\ExData\assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8535"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="20490" windowHeight="8540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Course Project 2: Plot 1 Timings</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>HP Omen (2.5Ghz i7, 16Gb RAM)</t>
+  </si>
+  <si>
+    <t>Macbook Pro (2.6Ghz i5, 8Gb RAM)</t>
   </si>
 </sst>
 </file>
@@ -403,18 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="26.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -422,13 +425,13 @@
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="2"/>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="3" t="s">
@@ -438,7 +441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="3" t="s">
@@ -448,7 +451,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -460,7 +463,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -472,7 +475,7 @@
         <v>34.75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -484,7 +487,7 @@
         <v>6.0000000000002274E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>3</v>
       </c>
@@ -496,7 +499,7 @@
         <v>11.86</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -508,18 +511,18 @@
         <v>0.39999999999999858</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>1</v>
       </c>
@@ -532,7 +535,7 @@
         <v>147.95201999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>2</v>
       </c>
@@ -545,7 +548,7 @@
         <v>0.24798000000004095</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>3</v>
       </c>
@@ -558,7 +561,7 @@
         <v>65.301599999999979</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -569,6 +572,59 @@
       <c r="D15" s="1">
         <f t="shared" si="1"/>
         <v>0.22914000000000101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>23.32</v>
+      </c>
+      <c r="D18">
+        <f>C18</f>
+        <v>23.32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>23.37</v>
+      </c>
+      <c r="D19">
+        <f>C19-C18</f>
+        <v>5.0000000000000711E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>33.65</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ref="D20:D21" si="2">C20-C19</f>
+        <v>10.279999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>33.74</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="2"/>
+        <v>9.0000000000003411E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>